<commit_message>
Generación del Estudio DT
</commit_message>
<xml_diff>
--- a/InfoCC.xlsx
+++ b/InfoCC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitHub\DTApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45B4422-A225-44FB-829F-589290B5D527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB108C3E-60FE-4759-826F-0CECA5CF42DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{750981B9-FDB2-499A-8017-7A783A86B903}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{750981B9-FDB2-499A-8017-7A783A86B903}"/>
   </bookViews>
   <sheets>
     <sheet name="PlanEstudios" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="103">
   <si>
     <t>Cod_Asignatura</t>
   </si>
@@ -335,6 +335,18 @@
   </si>
   <si>
     <t>Tipo</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Trabajo de Grado - Trabajos Investigativos</t>
+  </si>
+  <si>
+    <t>Trabajo de Grado - Asignaturas de Posgrado</t>
+  </si>
+  <si>
+    <t>Trabajo de Grado - Pasantías</t>
   </si>
 </sst>
 </file>
@@ -370,10 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -709,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEFCB4FA-7B45-421D-861F-C593BF1D698D}">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="A41" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,7 +756,7 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>4</v>
       </c>
       <c r="D2" t="s">
@@ -764,7 +773,7 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>4</v>
       </c>
       <c r="D3" t="s">
@@ -781,13 +790,13 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>4</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -798,13 +807,13 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -815,7 +824,7 @@
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>4</v>
       </c>
       <c r="D6" t="s">
@@ -832,10 +841,10 @@
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
@@ -852,7 +861,7 @@
       <c r="C8">
         <v>4</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>6</v>
       </c>
       <c r="E8" t="s">
@@ -869,7 +878,7 @@
       <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
@@ -886,7 +895,7 @@
       <c r="C10">
         <v>4</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" t="s">
         <v>6</v>
       </c>
       <c r="E10" t="s">
@@ -903,7 +912,7 @@
       <c r="C11">
         <v>4</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" t="s">
         <v>6</v>
       </c>
       <c r="E11" t="s">
@@ -920,7 +929,7 @@
       <c r="C12">
         <v>4</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" t="s">
         <v>6</v>
       </c>
       <c r="E12" t="s">
@@ -937,7 +946,7 @@
       <c r="C13">
         <v>4</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" t="s">
         <v>6</v>
       </c>
       <c r="E13" t="s">
@@ -954,7 +963,7 @@
       <c r="C14">
         <v>4</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" t="s">
         <v>6</v>
       </c>
       <c r="E14" t="s">
@@ -971,7 +980,7 @@
       <c r="C15">
         <v>4</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" t="s">
         <v>6</v>
       </c>
       <c r="E15" t="s">
@@ -1005,7 +1014,7 @@
       <c r="C17">
         <v>3</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" t="s">
         <v>32</v>
       </c>
       <c r="E17" t="s">
@@ -1022,7 +1031,7 @@
       <c r="C18">
         <v>3</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" t="s">
         <v>32</v>
       </c>
       <c r="E18" t="s">
@@ -1039,7 +1048,7 @@
       <c r="C19">
         <v>4</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" t="s">
         <v>32</v>
       </c>
       <c r="E19" t="s">
@@ -1056,7 +1065,7 @@
       <c r="C20">
         <v>3</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" t="s">
         <v>32</v>
       </c>
       <c r="E20" t="s">
@@ -1073,7 +1082,7 @@
       <c r="C21">
         <v>3</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" t="s">
         <v>32</v>
       </c>
       <c r="E21" t="s">
@@ -1107,7 +1116,7 @@
       <c r="C23">
         <v>3</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" t="s">
         <v>36</v>
       </c>
       <c r="E23" t="s">
@@ -1124,7 +1133,7 @@
       <c r="C24">
         <v>3</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" t="s">
         <v>36</v>
       </c>
       <c r="E24" t="s">
@@ -1141,7 +1150,7 @@
       <c r="C25">
         <v>3</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" t="s">
         <v>48</v>
       </c>
       <c r="E25" t="s">
@@ -1175,7 +1184,7 @@
       <c r="C27">
         <v>4</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" t="s">
         <v>48</v>
       </c>
       <c r="E27" t="s">
@@ -1192,7 +1201,7 @@
       <c r="C28">
         <v>4</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" t="s">
         <v>48</v>
       </c>
       <c r="E28" t="s">
@@ -1209,7 +1218,7 @@
       <c r="C29">
         <v>3</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" t="s">
         <v>48</v>
       </c>
       <c r="E29" t="s">
@@ -1226,7 +1235,7 @@
       <c r="C30">
         <v>3</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" t="s">
         <v>48</v>
       </c>
       <c r="E30" t="s">
@@ -1243,7 +1252,7 @@
       <c r="C31">
         <v>4</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" t="s">
         <v>48</v>
       </c>
       <c r="E31" t="s">
@@ -1260,7 +1269,7 @@
       <c r="C32">
         <v>4</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" t="s">
         <v>48</v>
       </c>
       <c r="E32" t="s">
@@ -1277,7 +1286,7 @@
       <c r="C33">
         <v>4</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" t="s">
         <v>48</v>
       </c>
       <c r="E33" t="s">
@@ -1294,7 +1303,7 @@
       <c r="C34">
         <v>4</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" t="s">
         <v>48</v>
       </c>
       <c r="E34" t="s">
@@ -1379,7 +1388,7 @@
       <c r="C39">
         <v>3</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" t="s">
         <v>54</v>
       </c>
       <c r="E39" t="s">
@@ -1396,7 +1405,7 @@
       <c r="C40">
         <v>3</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" t="s">
         <v>54</v>
       </c>
       <c r="E40" t="s">
@@ -1413,7 +1422,7 @@
       <c r="C41">
         <v>3</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" t="s">
         <v>54</v>
       </c>
       <c r="E41" t="s">
@@ -1430,7 +1439,7 @@
       <c r="C42">
         <v>3</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" t="s">
         <v>54</v>
       </c>
       <c r="E42" t="s">
@@ -1447,7 +1456,7 @@
       <c r="C43">
         <v>3</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" t="s">
         <v>54</v>
       </c>
       <c r="E43" t="s">
@@ -1481,7 +1490,7 @@
       <c r="C45">
         <v>4</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" t="s">
         <v>68</v>
       </c>
       <c r="E45" t="s">
@@ -1498,7 +1507,7 @@
       <c r="C46">
         <v>4</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" t="s">
         <v>68</v>
       </c>
       <c r="E46" t="s">
@@ -1515,7 +1524,7 @@
       <c r="C47">
         <v>4</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" t="s">
         <v>68</v>
       </c>
       <c r="E47" t="s">
@@ -1532,7 +1541,7 @@
       <c r="C48">
         <v>3</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" t="s">
         <v>68</v>
       </c>
       <c r="E48" t="s">
@@ -1549,7 +1558,7 @@
       <c r="C49">
         <v>4</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" t="s">
         <v>68</v>
       </c>
       <c r="E49" t="s">
@@ -1566,7 +1575,7 @@
       <c r="C50">
         <v>4</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" t="s">
         <v>68</v>
       </c>
       <c r="E50" t="s">
@@ -1583,7 +1592,7 @@
       <c r="C51">
         <v>4</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" t="s">
         <v>68</v>
       </c>
       <c r="E51" t="s">
@@ -1617,10 +1626,10 @@
       <c r="C53">
         <v>3</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" t="s">
         <v>84</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1634,10 +1643,10 @@
       <c r="C54">
         <v>4</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" t="s">
         <v>84</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E54" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1651,10 +1660,10 @@
       <c r="C55">
         <v>3</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" t="s">
         <v>84</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1668,10 +1677,10 @@
       <c r="C56">
         <v>3</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" t="s">
         <v>84</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1685,10 +1694,10 @@
       <c r="C57">
         <v>3</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" t="s">
         <v>84</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1702,10 +1711,10 @@
       <c r="C58">
         <v>4</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" t="s">
         <v>84</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E58" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1719,10 +1728,10 @@
       <c r="C59">
         <v>3</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" t="s">
         <v>84</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E59" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1736,10 +1745,10 @@
       <c r="C60">
         <v>3</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" t="s">
         <v>84</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E60" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1753,10 +1762,10 @@
       <c r="C61">
         <v>3</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" t="s">
         <v>84</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1770,10 +1779,10 @@
       <c r="C62">
         <v>4</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" t="s">
         <v>84</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1787,10 +1796,10 @@
       <c r="C63">
         <v>4</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" t="s">
         <v>84</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E63" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1804,10 +1813,10 @@
       <c r="C64">
         <v>4</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" t="s">
         <v>84</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E64" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1821,11 +1830,62 @@
       <c r="C65">
         <v>6</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" t="s">
         <v>84</v>
       </c>
-      <c r="E65" s="3" t="s">
-        <v>49</v>
+      <c r="E65" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>2027633</v>
+      </c>
+      <c r="B66" t="s">
+        <v>100</v>
+      </c>
+      <c r="C66">
+        <v>8</v>
+      </c>
+      <c r="D66" t="s">
+        <v>85</v>
+      </c>
+      <c r="E66" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>2027634</v>
+      </c>
+      <c r="B67" t="s">
+        <v>101</v>
+      </c>
+      <c r="C67">
+        <v>8</v>
+      </c>
+      <c r="D67" t="s">
+        <v>85</v>
+      </c>
+      <c r="E67" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>2027636</v>
+      </c>
+      <c r="B68" t="s">
+        <v>102</v>
+      </c>
+      <c r="C68">
+        <v>8</v>
+      </c>
+      <c r="D68" t="s">
+        <v>85</v>
+      </c>
+      <c r="E68" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1837,8 +1897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB17BBD5-D32D-472D-9D8F-E8840DAD6E18}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1864,7 +1924,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
@@ -1895,7 +1955,7 @@
       <c r="A4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4">
@@ -1923,7 +1983,7 @@
       <c r="A6" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>47</v>
       </c>
       <c r="C6">
@@ -1937,7 +1997,7 @@
       <c r="A7" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>47</v>
       </c>
       <c r="C7">
@@ -1948,10 +2008,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>47</v>
       </c>
       <c r="C8">
@@ -2000,7 +2060,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2045,10 +2105,10 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2">
         <v>2016377</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2059,10 +2119,10 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <v>2015556</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2073,10 +2133,10 @@
       <c r="B4" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4">
         <v>2015162</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2087,10 +2147,10 @@
       <c r="B5" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>2016342</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2101,10 +2161,10 @@
       <c r="B6" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>2015555</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2115,10 +2175,10 @@
       <c r="B7" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7">
         <v>2027310</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2129,10 +2189,10 @@
       <c r="B8" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8">
         <v>2019072</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Base de datos y extracción corregida
</commit_message>
<xml_diff>
--- a/InfoCC.xlsx
+++ b/InfoCC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitHub\DTApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB108C3E-60FE-4759-826F-0CECA5CF42DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A51EB5-BFE8-479F-8A49-C02ABE602910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{750981B9-FDB2-499A-8017-7A783A86B903}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{750981B9-FDB2-499A-8017-7A783A86B903}"/>
   </bookViews>
   <sheets>
     <sheet name="PlanEstudios" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="105">
   <si>
     <t>Cod_Asignatura</t>
   </si>
@@ -347,14 +347,28 @@
   </si>
   <si>
     <t>Trabajo de Grado - Pasantías</t>
+  </si>
+  <si>
+    <t>Fundamentos de Mecánica</t>
+  </si>
+  <si>
+    <t>Mecánica Newtoniana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -382,8 +396,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEFCB4FA-7B45-421D-861F-C593BF1D698D}">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1897,7 +1913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB17BBD5-D32D-472D-9D8F-E8840DAD6E18}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -2070,10 +2086,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180743DD-7D5E-4738-8A6D-0EB25F359AE2}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2130,7 +2146,7 @@
       <c r="A4">
         <v>1000006</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C4">
@@ -2194,6 +2210,20 @@
       </c>
       <c r="D8" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1000019</v>
+      </c>
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9">
+        <v>2015176</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arreglo de bugs, funciones centrales terminadas
</commit_message>
<xml_diff>
--- a/InfoCC.xlsx
+++ b/InfoCC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitHub\DTApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A51EB5-BFE8-479F-8A49-C02ABE602910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021FB1CC-D8E3-4292-A1D9-1868050A668F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{750981B9-FDB2-499A-8017-7A783A86B903}"/>
   </bookViews>
@@ -736,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEFCB4FA-7B45-421D-861F-C593BF1D698D}">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1914,7 +1914,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2086,10 +2086,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180743DD-7D5E-4738-8A6D-0EB25F359AE2}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2146,7 +2146,7 @@
       <c r="A4">
         <v>1000006</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C4">
@@ -2222,9 +2222,12 @@
       <c r="C9">
         <v>2015176</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>104</v>
       </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>